<commit_message>
update bug report for jumia app
</commit_message>
<xml_diff>
--- a/Jumia Bug Report/Jumia Bug Report.xlsx
+++ b/Jumia Bug Report/Jumia Bug Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ IDEA Community Edition 2024.1.4\java-projects\Automation Assessment - Paysky\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ IDEA Community Edition 2024.1.4\java-projects\Automation-Assessment-Paysky\Jumia Bug Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B060D417-9562-4E63-A583-6F74B72D94E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94D0A58-65A5-439A-8F5D-E58E18EF576B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{E022644B-76EC-4BBD-8E63-3AA410A8B5DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -207,6 +207,37 @@
   </si>
   <si>
     <t>The "Following" tab remains in English, while the rest of the interface is correctly translated into Arabic.</t>
+  </si>
+  <si>
+    <t>BUG_SearchFunctionality_06</t>
+  </si>
+  <si>
+    <t>Unrelated products displayed when searching for "laptop" in Arabic</t>
+  </si>
+  <si>
+    <t>When performing a search using the Arabic word for "laptop" (لاب توب), some unrelated products are displayed in the search results. The displayed items do not align with the intended search query for laptop-related products, leading to a confusing user experience</t>
+  </si>
+  <si>
+    <t>Go to the website’s main search bar.
+Enter the Arabic word "لاب توب" (the Arabic term for "laptop") into the search bar.
+Press Enter or click the search icon.
+Observe the products listed in the search results.</t>
+  </si>
+  <si>
+    <t>Only laptop-related products or accessories relevant to the search query "لاب توب" should appear in the search results.</t>
+  </si>
+  <si>
+    <t>Some products displayed in the search results are not related to laptops or laptop accessories, such as unrelated electronics or other categories of products.</t>
+  </si>
+  <si>
+    <t>TC_SearchFunctionality_Arabic_01</t>
+  </si>
+  <si>
+    <t>Oppo a 76, 
+Android 13.0, Jumia App Version 16.4.1</t>
+  </si>
+  <si>
+    <t>The search functionality should accurately interpret Arabic terms and display relevant results, especially for commonly searched items like laptops. This issue may affect Arabic-speaking users’ ability to find desired products quickly.</t>
   </si>
 </sst>
 </file>
@@ -533,6 +564,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>23621</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>933450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FAB2A3C-A6BB-4C00-9E1C-B207275B790A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="59488196" y="5772150"/>
+          <a:ext cx="1157479" cy="923925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -833,15 +914,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9850E0-615D-4654-805D-10A168A37C74}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="80.85546875" customWidth="1"/>
     <col min="3" max="3" width="186.42578125" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" customWidth="1"/>
@@ -1106,6 +1187,47 @@
         <v>48</v>
       </c>
     </row>
+    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>